<commit_message>
Latest Changes - 28 Mar 2023
</commit_message>
<xml_diff>
--- a/TestData/T1886_Companies_CompanyDetailsPage_CompanyFinancials_EditAndDelete.xlsx
+++ b/TestData/T1886_Companies_CompanyDetailsPage_CompanyFinancials_EditAndDelete.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hgandhi1012\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202B39D2-F05E-4AB4-A223-DB3D83F620E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7536" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>CompanyType</t>
   </si>
@@ -46,9 +47,6 @@
     <t>StandardTestCompany</t>
   </si>
   <si>
-    <t>Capital Provider</t>
-  </si>
-  <si>
     <t>CompanyFinancialLabel</t>
   </si>
   <si>
@@ -59,9 +57,6 @@
   </si>
   <si>
     <t>CompanyDetailTitle</t>
-  </si>
-  <si>
-    <t>CapProviderTestCompany</t>
   </si>
   <si>
     <t>UpdateYear</t>
@@ -94,7 +89,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -415,11 +410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,10 +439,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -470,14 +465,6 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -487,11 +474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,39 +489,39 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -544,11 +531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +550,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Companies Final - 11 Jan 2024
</commit_message>
<xml_diff>
--- a/TestData/T1886_Companies_CompanyDetailsPage_CompanyFinancials_EditAndDelete.xlsx
+++ b/TestData/T1886_Companies_CompanyDetailsPage_CompanyFinancials_EditAndDelete.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D2FD2A-33D6-4A20-8C52-F4391429B557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CE9264-34E0-4536-88B2-AAE02DCDA987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" r:id="rId1"/>
@@ -68,22 +68,22 @@
     <t>NoRecordMsg</t>
   </si>
   <si>
-    <t>2025</t>
-  </si>
-  <si>
-    <t>2024</t>
-  </si>
-  <si>
-    <t>2023</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
     <t>2021</t>
   </si>
   <si>
     <t>Drew Koecher</t>
+  </si>
+  <si>
+    <t>2030</t>
+  </si>
+  <si>
+    <t>2029</t>
+  </si>
+  <si>
+    <t>2028</t>
+  </si>
+  <si>
+    <t>2027</t>
   </si>
 </sst>
 </file>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,28 +500,28 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -534,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -550,7 +550,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>